<commit_message>
Commit by Farheen: Changes done in company, item , unit and Indent.
</commit_message>
<xml_diff>
--- a/InVanWebApp/ExcelFileFormat/Download-Format-Company.xlsx
+++ b/InVanWebApp/ExcelFileFormat/Download-Format-Company.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\InventoryManagement_VangiFoods_V2\InventoryManagement_VangiFoods_V2\InVanWebApp\ExcelFileFormat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12789BE4-EBC4-473B-9D27-34F8A8B58C9E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF124F8-0544-4770-B3B3-7C362D344BC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{6F127CB0-B9FF-4DB5-986B-8D945220DED4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>TM_0001</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>IsBlackListed</t>
+  </si>
+  <si>
+    <t>Anand,Vadodara</t>
   </si>
 </sst>
 </file>
@@ -136,67 +139,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -550,7 +493,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,22 +558,25 @@
       <c r="E2">
         <v>9854213615</v>
       </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
       <c r="I2" t="b">
         <v>1</v>
       </c>
       <c r="J2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>